<commit_message>
GC files moved back to cl folder
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/CriteriaTaxonomy-V1.0.3.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/CriteriaTaxonomy-V1.0.3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="EG-Convictions" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2331" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2337" uniqueCount="354">
   <si>
     <t>005eb9ed-1347-4ca3-bb29-9bc0db64e1ab</t>
   </si>
@@ -1105,13 +1105,19 @@
   </si>
   <si>
     <t>Beware that in version 1.0.2 this UUID is not consistent with the structure. It should have been 30450436-f559-4dfa-98ba-f0842ed9d2a0 from the very beginning as it identifes the same structure as the one in criterion CRITERION.EXCLUSION.CONFLICT_OF_INTEREST.PROCEDURE_PARTICIPATION</t>
+  </si>
+  <si>
+    <t>f4978772-3126-4ded-bc30-f50da8c3a038</t>
+  </si>
+  <si>
+    <t>This UUID has been changed as per 20180430th. To distinguish this subgroup from those other containing the same questions but different Property Group Type Code (ON*, instead of ONTRUE).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1282,6 +1288,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="38">
@@ -1709,7 +1721,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1766,6 +1778,9 @@
     <xf numFmtId="0" fontId="19" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="96">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2165,9 +2180,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q127"/>
+  <dimension ref="A1:R127"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2182,7 +2197,7 @@
     <col min="18" max="16384" width="10.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>5</v>
       </c>
@@ -2232,7 +2247,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="22">
         <v>1</v>
       </c>
@@ -2264,7 +2279,7 @@
       </c>
       <c r="Q2" s="25"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>1</v>
       </c>
@@ -2282,7 +2297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>1</v>
       </c>
@@ -2306,7 +2321,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>1</v>
       </c>
@@ -2334,7 +2349,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <v>1</v>
       </c>
@@ -2363,7 +2378,7 @@
       <c r="P6" s="27"/>
       <c r="Q6" s="6"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>1</v>
       </c>
@@ -2392,7 +2407,7 @@
       <c r="P7" s="27"/>
       <c r="Q7" s="6"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>1</v>
       </c>
@@ -2421,7 +2436,7 @@
       <c r="P8" s="27"/>
       <c r="Q8" s="6"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <v>1</v>
       </c>
@@ -2450,7 +2465,7 @@
       <c r="P9" s="27"/>
       <c r="Q9" s="6"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>1</v>
       </c>
@@ -2470,14 +2485,17 @@
       <c r="M10" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="N10" s="21" t="s">
-        <v>26</v>
+      <c r="N10" s="30" t="s">
+        <v>352</v>
       </c>
       <c r="O10" s="27"/>
       <c r="P10" s="27"/>
       <c r="Q10" s="27"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10" s="30" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>1</v>
       </c>
@@ -2509,7 +2527,7 @@
       <c r="P11" s="27"/>
       <c r="Q11" s="27"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>1</v>
       </c>
@@ -2541,7 +2559,7 @@
       </c>
       <c r="Q12" s="27"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <v>1</v>
       </c>
@@ -2576,7 +2594,7 @@
       <c r="P13" s="27"/>
       <c r="Q13" s="27"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <v>1</v>
       </c>
@@ -2594,7 +2612,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <v>1</v>
       </c>
@@ -2618,7 +2636,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <v>1</v>
       </c>
@@ -2642,7 +2660,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
         <v>1</v>
       </c>
@@ -2669,7 +2687,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="21">
         <v>1</v>
       </c>
@@ -2696,7 +2714,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>1</v>
       </c>
@@ -2723,7 +2741,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>2</v>
       </c>
@@ -2755,7 +2773,7 @@
       </c>
       <c r="Q20" s="24"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="21">
         <v>2</v>
       </c>
@@ -2773,7 +2791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="21">
         <v>2</v>
       </c>
@@ -2797,7 +2815,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
         <v>2</v>
       </c>
@@ -2825,7 +2843,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="21">
         <v>2</v>
       </c>
@@ -2854,7 +2872,7 @@
       <c r="P24" s="27"/>
       <c r="Q24" s="6"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="21">
         <v>2</v>
       </c>
@@ -2883,7 +2901,7 @@
       <c r="P25" s="27"/>
       <c r="Q25" s="6"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="21">
         <v>2</v>
       </c>
@@ -2912,7 +2930,7 @@
       <c r="P26" s="27"/>
       <c r="Q26" s="6"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="21">
         <v>2</v>
       </c>
@@ -2941,7 +2959,7 @@
       <c r="P27" s="27"/>
       <c r="Q27" s="6"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="21">
         <v>2</v>
       </c>
@@ -2961,14 +2979,17 @@
       <c r="M28" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="N28" s="21" t="s">
-        <v>26</v>
+      <c r="N28" s="30" t="s">
+        <v>352</v>
       </c>
       <c r="O28" s="27"/>
       <c r="P28" s="27"/>
       <c r="Q28" s="27"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R28" s="30" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="21">
         <v>2</v>
       </c>
@@ -3000,7 +3021,7 @@
       <c r="P29" s="27"/>
       <c r="Q29" s="27"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="21">
         <v>2</v>
       </c>
@@ -3032,7 +3053,7 @@
       </c>
       <c r="Q30" s="27"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="21">
         <v>2</v>
       </c>
@@ -3067,7 +3088,7 @@
       <c r="P31" s="27"/>
       <c r="Q31" s="27"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="21">
         <v>2</v>
       </c>
@@ -3085,7 +3106,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="21">
         <v>2</v>
       </c>
@@ -3109,7 +3130,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="21">
         <v>2</v>
       </c>
@@ -3133,7 +3154,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="21">
         <v>2</v>
       </c>
@@ -3160,7 +3181,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="21">
         <v>2</v>
       </c>
@@ -3187,7 +3208,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="20">
         <v>2</v>
       </c>
@@ -3214,7 +3235,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <v>3</v>
       </c>
@@ -3246,7 +3267,7 @@
       </c>
       <c r="Q38" s="24"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="20">
         <v>3</v>
       </c>
@@ -3264,7 +3285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="20">
         <v>3</v>
       </c>
@@ -3288,7 +3309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="20">
         <v>3</v>
       </c>
@@ -3316,7 +3337,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="20">
         <v>3</v>
       </c>
@@ -3345,7 +3366,7 @@
       <c r="P42" s="27"/>
       <c r="Q42" s="6"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="20">
         <v>3</v>
       </c>
@@ -3374,7 +3395,7 @@
       <c r="P43" s="27"/>
       <c r="Q43" s="6"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="20">
         <v>3</v>
       </c>
@@ -3403,7 +3424,7 @@
       <c r="P44" s="27"/>
       <c r="Q44" s="6"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="20">
         <v>3</v>
       </c>
@@ -3432,7 +3453,7 @@
       <c r="P45" s="27"/>
       <c r="Q45" s="6"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="20">
         <v>3</v>
       </c>
@@ -3452,14 +3473,17 @@
       <c r="M46" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="N46" s="21" t="s">
-        <v>26</v>
+      <c r="N46" s="30" t="s">
+        <v>352</v>
       </c>
       <c r="O46" s="27"/>
       <c r="P46" s="27"/>
       <c r="Q46" s="27"/>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R46" s="30" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="20">
         <v>3</v>
       </c>
@@ -3491,7 +3515,7 @@
       <c r="P47" s="27"/>
       <c r="Q47" s="27"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="20">
         <v>3</v>
       </c>
@@ -3523,7 +3547,7 @@
       </c>
       <c r="Q48" s="27"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="20">
         <v>3</v>
       </c>
@@ -3558,7 +3582,7 @@
       <c r="P49" s="27"/>
       <c r="Q49" s="27"/>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="20">
         <v>3</v>
       </c>
@@ -3576,7 +3600,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="20">
         <v>3</v>
       </c>
@@ -3600,7 +3624,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="20">
         <v>3</v>
       </c>
@@ -3624,7 +3648,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="20">
         <v>3</v>
       </c>
@@ -3651,7 +3675,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="20">
         <v>3</v>
       </c>
@@ -3678,7 +3702,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="20">
         <v>3</v>
       </c>
@@ -3705,7 +3729,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="17">
         <v>4</v>
       </c>
@@ -3737,7 +3761,7 @@
       </c>
       <c r="Q56" s="24"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="20">
         <v>4</v>
       </c>
@@ -3755,7 +3779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="20">
         <v>4</v>
       </c>
@@ -3779,7 +3803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="20">
         <v>4</v>
       </c>
@@ -3807,7 +3831,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="20">
         <v>4</v>
       </c>
@@ -3836,7 +3860,7 @@
       <c r="P60" s="27"/>
       <c r="Q60" s="6"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="20">
         <v>4</v>
       </c>
@@ -3865,7 +3889,7 @@
       <c r="P61" s="27"/>
       <c r="Q61" s="6"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="20">
         <v>4</v>
       </c>
@@ -3894,7 +3918,7 @@
       <c r="P62" s="27"/>
       <c r="Q62" s="6"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="20">
         <v>4</v>
       </c>
@@ -3923,7 +3947,7 @@
       <c r="P63" s="27"/>
       <c r="Q63" s="6"/>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="20">
         <v>4</v>
       </c>
@@ -3943,12 +3967,15 @@
       <c r="M64" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="N64" s="21" t="s">
-        <v>26</v>
+      <c r="N64" s="30" t="s">
+        <v>352</v>
       </c>
       <c r="O64" s="27"/>
       <c r="P64" s="27"/>
       <c r="Q64" s="27"/>
+      <c r="R64" s="30" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="20">
@@ -4385,7 +4412,7 @@
       <c r="P80" s="27"/>
       <c r="Q80" s="6"/>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="20">
         <v>5</v>
       </c>
@@ -4414,7 +4441,7 @@
       <c r="P81" s="27"/>
       <c r="Q81" s="6"/>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="20">
         <v>5</v>
       </c>
@@ -4434,14 +4461,17 @@
       <c r="M82" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="N82" s="21" t="s">
-        <v>26</v>
+      <c r="N82" s="30" t="s">
+        <v>352</v>
       </c>
       <c r="O82" s="27"/>
       <c r="P82" s="27"/>
       <c r="Q82" s="27"/>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R82" s="30" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="20">
         <v>5</v>
       </c>
@@ -4473,7 +4503,7 @@
       <c r="P83" s="27"/>
       <c r="Q83" s="27"/>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="20">
         <v>5</v>
       </c>
@@ -4505,7 +4535,7 @@
       </c>
       <c r="Q84" s="27"/>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="20">
         <v>5</v>
       </c>
@@ -4540,7 +4570,7 @@
       <c r="P85" s="27"/>
       <c r="Q85" s="27"/>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="20">
         <v>5</v>
       </c>
@@ -4558,7 +4588,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="20">
         <v>5</v>
       </c>
@@ -4582,7 +4612,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="20">
         <v>5</v>
       </c>
@@ -4606,7 +4636,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="20">
         <v>5</v>
       </c>
@@ -4633,7 +4663,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="20">
         <v>5</v>
       </c>
@@ -4660,7 +4690,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="20">
         <v>5</v>
       </c>
@@ -4687,7 +4717,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="17">
         <v>6</v>
       </c>
@@ -4719,7 +4749,7 @@
       </c>
       <c r="Q92" s="24"/>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="20">
         <v>6</v>
       </c>
@@ -4737,7 +4767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="20">
         <v>6</v>
       </c>
@@ -4761,7 +4791,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="20">
         <v>6</v>
       </c>
@@ -4789,7 +4819,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" s="20">
         <v>6</v>
       </c>
@@ -4818,7 +4848,7 @@
       <c r="P96" s="27"/>
       <c r="Q96" s="6"/>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="20">
         <v>6</v>
       </c>
@@ -4847,7 +4877,7 @@
       <c r="P97" s="27"/>
       <c r="Q97" s="6"/>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="20">
         <v>6</v>
       </c>
@@ -4876,7 +4906,7 @@
       <c r="P98" s="27"/>
       <c r="Q98" s="6"/>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="20">
         <v>6</v>
       </c>
@@ -4905,7 +4935,7 @@
       <c r="P99" s="27"/>
       <c r="Q99" s="6"/>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="20">
         <v>6</v>
       </c>
@@ -4925,14 +4955,17 @@
       <c r="M100" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="N100" s="21" t="s">
-        <v>26</v>
+      <c r="N100" s="30" t="s">
+        <v>352</v>
       </c>
       <c r="O100" s="27"/>
       <c r="P100" s="27"/>
       <c r="Q100" s="27"/>
-    </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R100" s="30" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="20">
         <v>6</v>
       </c>
@@ -4964,7 +4997,7 @@
       <c r="P101" s="27"/>
       <c r="Q101" s="27"/>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="20">
         <v>6</v>
       </c>
@@ -4996,7 +5029,7 @@
       </c>
       <c r="Q102" s="27"/>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" s="20">
         <v>6</v>
       </c>
@@ -5031,7 +5064,7 @@
       <c r="P103" s="27"/>
       <c r="Q103" s="27"/>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" s="20">
         <v>6</v>
       </c>
@@ -5049,7 +5082,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="20">
         <v>6</v>
       </c>
@@ -5073,7 +5106,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="20">
         <v>6</v>
       </c>
@@ -5097,7 +5130,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="20">
         <v>6</v>
       </c>
@@ -5124,7 +5157,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" s="20">
         <v>6</v>
       </c>
@@ -5151,7 +5184,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" s="20">
         <v>6</v>
       </c>
@@ -5178,7 +5211,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="110" spans="1:17" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:18" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="19"/>
       <c r="B110" s="19"/>
       <c r="C110" s="19"/>
@@ -6507,7 +6540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9081,7 +9114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10583,9 +10616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16935,12 +16966,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="11" width="4.42578125" style="18" customWidth="1"/>
-    <col min="12" max="16384" width="11.5703125" style="18"/>
+    <col min="12" max="12" width="29.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.5703125" style="18" customWidth="1"/>
+    <col min="14" max="14" width="38.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="11.5703125" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -18147,7 +18181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -20671,7 +20705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -21526,9 +21560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>